<commit_message>
Generated the Parser and optimized the code
</commit_message>
<xml_diff>
--- a/new/data.xlsx
+++ b/new/data.xlsx
@@ -1,38 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edu/PycharmProjects/IA_final_project/new/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730AE2C9-90E3-DA44-89E0-C547D271AB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Heating" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Cooling" sheetId="2" r:id="rId5"/>
+    <sheet name="Heating" sheetId="1" r:id="rId1"/>
+    <sheet name="Cooling" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -41,126 +70,138 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="9">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -350,83 +391,88 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="20" width="4.0"/>
+    <col min="2" max="20" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2">
         <v>16.5</v>
       </c>
       <c r="D1" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2">
         <v>17.5</v>
       </c>
       <c r="F1" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2">
         <v>18.5</v>
       </c>
       <c r="H1" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2">
         <v>19.5</v>
       </c>
       <c r="J1" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2">
         <v>20.5</v>
       </c>
       <c r="L1" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="M1" s="2">
         <v>21.5</v>
       </c>
       <c r="N1" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="O1" s="2">
         <v>22.5</v>
       </c>
       <c r="P1" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="2">
         <v>23.5</v>
       </c>
       <c r="R1" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="S1" s="2">
         <v>24.5</v>
       </c>
       <c r="T1" s="3">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <f t="array" ref="A2:A20">TRANSPOSE(B1:T1)</f>
         <v>16</v>
@@ -440,9 +486,10 @@
       <c r="D2" s="5">
         <v>0.2</v>
       </c>
+      <c r="E2" s="16"/>
       <c r="T2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>16.5</v>
       </c>
@@ -460,9 +507,9 @@
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5">
         <v>0.1</v>
@@ -478,7 +525,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>17.5</v>
       </c>
@@ -496,9 +543,9 @@
       </c>
       <c r="T5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="E6" s="5">
         <v>0.1</v>
@@ -514,7 +561,7 @@
       </c>
       <c r="T6" s="6"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>18.5</v>
       </c>
@@ -532,9 +579,9 @@
       </c>
       <c r="T7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5">
         <v>0.1</v>
@@ -550,7 +597,7 @@
       </c>
       <c r="T8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>19.5</v>
       </c>
@@ -568,9 +615,9 @@
       </c>
       <c r="T9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5">
         <v>0.1</v>
@@ -586,7 +633,7 @@
       </c>
       <c r="T10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>20.5</v>
       </c>
@@ -604,9 +651,9 @@
       </c>
       <c r="T11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K12" s="5">
         <v>0.1</v>
@@ -622,7 +669,7 @@
       </c>
       <c r="T12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>21.5</v>
       </c>
@@ -640,9 +687,9 @@
       </c>
       <c r="T13" s="6"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="M14" s="5">
         <v>0.1</v>
@@ -658,7 +705,7 @@
       </c>
       <c r="T14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>22.5</v>
       </c>
@@ -676,9 +723,9 @@
       </c>
       <c r="T15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="O16" s="5">
         <v>0.1</v>
@@ -694,7 +741,7 @@
       </c>
       <c r="T16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>23.5</v>
       </c>
@@ -712,9 +759,9 @@
       </c>
       <c r="T17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="Q18" s="5">
         <v>0.1</v>
@@ -725,11 +772,11 @@
       <c r="S18" s="5">
         <v>0.5</v>
       </c>
-      <c r="T18" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="T18" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>24.5</v>
       </c>
@@ -739,118 +786,119 @@
       <c r="S19" s="5">
         <v>0.2</v>
       </c>
-      <c r="T19" s="7">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="8">
-        <v>25.0</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="T20" s="11">
+      <c r="T19" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="T20" s="9">
         <v>0.9</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="24" width="5.13"/>
+    <col min="1" max="24" width="5.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13">
-        <v>16.0</v>
-      </c>
-      <c r="C1" s="13">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11">
+        <v>16</v>
+      </c>
+      <c r="C1" s="11">
         <v>16.5</v>
       </c>
-      <c r="D1" s="13">
-        <v>17.0</v>
-      </c>
-      <c r="E1" s="13">
+      <c r="D1" s="11">
+        <v>17</v>
+      </c>
+      <c r="E1" s="11">
         <v>17.5</v>
       </c>
-      <c r="F1" s="13">
-        <v>18.0</v>
-      </c>
-      <c r="G1" s="13">
+      <c r="F1" s="11">
+        <v>18</v>
+      </c>
+      <c r="G1" s="11">
         <v>18.5</v>
       </c>
-      <c r="H1" s="13">
-        <v>19.0</v>
-      </c>
-      <c r="I1" s="13">
+      <c r="H1" s="11">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11">
         <v>19.5</v>
       </c>
-      <c r="J1" s="13">
-        <v>20.0</v>
-      </c>
-      <c r="K1" s="13">
+      <c r="J1" s="11">
+        <v>20</v>
+      </c>
+      <c r="K1" s="11">
         <v>20.5</v>
       </c>
-      <c r="L1" s="13">
-        <v>21.0</v>
-      </c>
-      <c r="M1" s="13">
+      <c r="L1" s="11">
+        <v>21</v>
+      </c>
+      <c r="M1" s="11">
         <v>21.5</v>
       </c>
-      <c r="N1" s="13">
-        <v>22.0</v>
-      </c>
-      <c r="O1" s="13">
+      <c r="N1" s="11">
+        <v>22</v>
+      </c>
+      <c r="O1" s="11">
         <v>22.5</v>
       </c>
-      <c r="P1" s="13">
-        <v>23.0</v>
-      </c>
-      <c r="Q1" s="13">
+      <c r="P1" s="11">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="11">
         <v>23.5</v>
       </c>
-      <c r="R1" s="13">
-        <v>24.0</v>
-      </c>
-      <c r="S1" s="13">
+      <c r="R1" s="11">
+        <v>24</v>
+      </c>
+      <c r="S1" s="11">
         <v>24.5</v>
       </c>
-      <c r="T1" s="14">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="15">
+      <c r="T1" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="13">
         <f t="array" ref="A2:A20">TRANSPOSE(B1:T1)</f>
         <v>16</v>
       </c>
@@ -862,8 +910,8 @@
       </c>
       <c r="T2" s="6"/>
     </row>
-    <row r="3">
-      <c r="A3" s="15">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="13">
         <v>16.5</v>
       </c>
       <c r="B3" s="5">
@@ -877,9 +925,9 @@
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4">
-      <c r="A4" s="15">
-        <v>17.0</v>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="13">
+        <v>17</v>
       </c>
       <c r="C4" s="5">
         <v>0.7</v>
@@ -891,10 +939,10 @@
         <v>0.1</v>
       </c>
       <c r="T4" s="6"/>
-      <c r="X4" s="16"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="15">
+      <c r="X4" s="14"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="13">
         <v>17.5</v>
       </c>
       <c r="D5" s="5">
@@ -908,9 +956,9 @@
       </c>
       <c r="T5" s="6"/>
     </row>
-    <row r="6">
-      <c r="A6" s="15">
-        <v>18.0</v>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="13">
+        <v>18</v>
       </c>
       <c r="E6" s="5">
         <v>0.7</v>
@@ -923,8 +971,8 @@
       </c>
       <c r="T6" s="6"/>
     </row>
-    <row r="7">
-      <c r="A7" s="15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="13">
         <v>18.5</v>
       </c>
       <c r="F7" s="5">
@@ -938,9 +986,9 @@
       </c>
       <c r="T7" s="6"/>
     </row>
-    <row r="8">
-      <c r="A8" s="15">
-        <v>19.0</v>
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="13">
+        <v>19</v>
       </c>
       <c r="G8" s="5">
         <v>0.7</v>
@@ -953,8 +1001,8 @@
       </c>
       <c r="T8" s="6"/>
     </row>
-    <row r="9">
-      <c r="A9" s="15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="13">
         <v>19.5</v>
       </c>
       <c r="H9" s="5">
@@ -968,9 +1016,9 @@
       </c>
       <c r="T9" s="6"/>
     </row>
-    <row r="10">
-      <c r="A10" s="15">
-        <v>20.0</v>
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="13">
+        <v>20</v>
       </c>
       <c r="I10" s="5">
         <v>0.7</v>
@@ -983,8 +1031,8 @@
       </c>
       <c r="T10" s="6"/>
     </row>
-    <row r="11">
-      <c r="A11" s="15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="13">
         <v>20.5</v>
       </c>
       <c r="J11" s="5">
@@ -998,9 +1046,9 @@
       </c>
       <c r="T11" s="6"/>
     </row>
-    <row r="12">
-      <c r="A12" s="15">
-        <v>21.0</v>
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="13">
+        <v>21</v>
       </c>
       <c r="K12" s="5">
         <v>0.7</v>
@@ -1013,8 +1061,8 @@
       </c>
       <c r="T12" s="6"/>
     </row>
-    <row r="13">
-      <c r="A13" s="15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13">
         <v>21.5</v>
       </c>
       <c r="L13" s="5">
@@ -1028,9 +1076,9 @@
       </c>
       <c r="T13" s="6"/>
     </row>
-    <row r="14">
-      <c r="A14" s="15">
-        <v>22.0</v>
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13">
+        <v>22</v>
       </c>
       <c r="M14" s="5">
         <v>0.7</v>
@@ -1043,8 +1091,8 @@
       </c>
       <c r="T14" s="6"/>
     </row>
-    <row r="15">
-      <c r="A15" s="15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13">
         <v>22.5</v>
       </c>
       <c r="N15" s="5">
@@ -1058,9 +1106,9 @@
       </c>
       <c r="T15" s="6"/>
     </row>
-    <row r="16">
-      <c r="A16" s="15">
-        <v>23.0</v>
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="13">
+        <v>23</v>
       </c>
       <c r="O16" s="5">
         <v>0.7</v>
@@ -1073,10 +1121,10 @@
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="7"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="15">
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="13">
         <v>23.5</v>
       </c>
       <c r="P17" s="5">
@@ -1089,11 +1137,11 @@
         <v>0.1</v>
       </c>
       <c r="S17" s="5"/>
-      <c r="T17" s="7"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="15">
-        <v>24.0</v>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="13">
+        <v>24</v>
       </c>
       <c r="Q18" s="5">
         <v>0.7</v>
@@ -1104,16 +1152,16 @@
       <c r="S18" s="5">
         <v>0.1</v>
       </c>
-      <c r="T18" s="7"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="15">
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="13">
         <v>24.5</v>
       </c>
-      <c r="R19" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="S19" s="17">
+      <c r="R19" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="S19" s="5">
         <v>0.2</v>
       </c>
       <c r="T19" s="6">
@@ -1121,39 +1169,39 @@
       </c>
       <c r="X19" s="5"/>
     </row>
-    <row r="20">
-      <c r="A20" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="T20" s="19">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="15">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="T20" s="9">
         <v>0.3</v>
       </c>
       <c r="X20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="X21" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>